<commit_message>
Casey's template spreadsheet of 10/18/23, version 2
</commit_message>
<xml_diff>
--- a/xlsx/template-spreadsheet.xlsx
+++ b/xlsx/template-spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ctpstemp-my.sharepoint.com/personal/ccooper_ctps_org/Documents/Desktop/Bicycle and Pedestrian Count Database Update/Count Data Formatting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{A3ED7B84-BEE4-4881-9961-112816DF7AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1960685-433E-46DD-A0FC-BDF5333672A8}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{A3ED7B84-BEE4-4881-9961-112816DF7AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D130C5D-A817-486F-A19A-1EAC40109E4D}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="390" windowWidth="21240" windowHeight="14985" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="19180" windowHeight="10340" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="445">
   <si>
     <t>Municipality</t>
   </si>
@@ -1123,14 +1134,290 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Bicycle/Pedestrian Facility Name
+</t>
+    </r>
+    <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
+        <i/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>(if applicable)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ashland</t>
+  </si>
+  <si>
+    <t>Bellingham</t>
+  </si>
+  <si>
+    <t>Beverly</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>Boxborough</t>
+  </si>
+  <si>
+    <t>Braintree</t>
+  </si>
+  <si>
+    <t>Burlington</t>
+  </si>
+  <si>
+    <t>Canton</t>
+  </si>
+  <si>
+    <t>Carlisle</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Cohasset</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>Danvers</t>
+  </si>
+  <si>
+    <t>Dedham</t>
+  </si>
+  <si>
+    <t>Dover</t>
+  </si>
+  <si>
+    <t>Essex</t>
+  </si>
+  <si>
+    <t>Foxborough</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Hingham</t>
+  </si>
+  <si>
+    <t>Holbrook</t>
+  </si>
+  <si>
+    <t>Holliston</t>
+  </si>
+  <si>
+    <t>Hopkinton</t>
+  </si>
+  <si>
+    <t>Hull</t>
+  </si>
+  <si>
+    <t>Ipswich</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Littleton</t>
+  </si>
+  <si>
+    <t>Lynn</t>
+  </si>
+  <si>
+    <t>Lynnfield</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Marshfield</t>
+  </si>
+  <si>
+    <t>Maynard</t>
+  </si>
+  <si>
+    <t>Medfield</t>
+  </si>
+  <si>
+    <t>Medway</t>
+  </si>
+  <si>
+    <t>Melrose</t>
+  </si>
+  <si>
+    <t>Middleton</t>
+  </si>
+  <si>
+    <t>Millis</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>Nahant</t>
+  </si>
+  <si>
+    <t>Natick</t>
+  </si>
+  <si>
+    <t>Norfolk</t>
+  </si>
+  <si>
+    <t>North Reading</t>
+  </si>
+  <si>
+    <t>Norwell</t>
+  </si>
+  <si>
+    <t>Norwood</t>
+  </si>
+  <si>
+    <t>Peabody</t>
+  </si>
+  <si>
+    <t>Randolph</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Rockland</t>
+  </si>
+  <si>
+    <t>Rockport</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Saugus</t>
+  </si>
+  <si>
+    <t>Scituate</t>
+  </si>
+  <si>
+    <t>Sharon</t>
+  </si>
+  <si>
+    <t>Sherborn</t>
+  </si>
+  <si>
+    <t>Southborough</t>
+  </si>
+  <si>
+    <t>Stoneham</t>
+  </si>
+  <si>
+    <t>Stow</t>
+  </si>
+  <si>
+    <t>Sudbury</t>
+  </si>
+  <si>
+    <t>Swampscott</t>
+  </si>
+  <si>
+    <t>Topsfield</t>
+  </si>
+  <si>
+    <t>Walpole</t>
+  </si>
+  <si>
+    <t>Wayland</t>
+  </si>
+  <si>
+    <t>Wellesley</t>
+  </si>
+  <si>
+    <t>Wenham</t>
+  </si>
+  <si>
+    <t>Weston</t>
+  </si>
+  <si>
+    <t>Westwood</t>
+  </si>
+  <si>
+    <t>Weymouth</t>
+  </si>
+  <si>
+    <t>Wilmington</t>
+  </si>
+  <si>
+    <t>Winchester</t>
+  </si>
+  <si>
+    <t>Winthrop</t>
+  </si>
+  <si>
+    <t>Woburn</t>
+  </si>
+  <si>
+    <t>Wrentham</t>
+  </si>
+  <si>
+    <t>Bicycle/Pedestrian Facility Segment</t>
+  </si>
+  <si>
+    <t>Bicycle/Pedestrian Facility Intersection</t>
+  </si>
+  <si>
+    <t>Street Segment</t>
+  </si>
+  <si>
+    <t>Street Intersection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other (please type in cell to the right)</t>
+  </si>
+  <si>
+    <t>Other (please type in cell to the right)</t>
+  </si>
+  <si>
+    <t>Other (please type in cell below)</t>
+  </si>
+  <si>
+    <t>Bicycle/Pedestrian Facility Name</t>
+  </si>
+  <si>
+    <t>Arthur Fiedler Footbridge</t>
+  </si>
+  <si>
+    <t>Dr. Paul Dudley White Path</t>
+  </si>
+  <si>
+    <t>Salem-Marblehead Trail</t>
+  </si>
+  <si>
+    <t>Southern New England Trunkline Trail</t>
+  </si>
+  <si>
+    <t>Southwest Corridor Park</t>
+  </si>
+  <si>
+    <t>Cleveland Circle - Chestnut Hill Ave at Beacon St</t>
+  </si>
+  <si>
+    <t>Sweetser Circle - Broadway and Bartlett Street</t>
+  </si>
+  <si>
+    <t>Union Square - Washington St between Kingman Rd and Hawkins St</t>
+  </si>
+  <si>
+    <t>Webster Square - Park Avenue at Mill Street</t>
+  </si>
+  <si>
+    <t>Western Avenue Bridge at Memorial Drive</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Street #2
 </t>
     </r>
@@ -1171,292 +1458,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please select from the drop-down menus below</t>
+      <t>Please select from the drop-down menus below, when applicable.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Bicycle/Pedestrian Facility Name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(if applicable)</t>
-    </r>
-  </si>
-  <si>
-    <t>Ashland</t>
-  </si>
-  <si>
-    <t>Bellingham</t>
-  </si>
-  <si>
-    <t>Beverly</t>
-  </si>
-  <si>
-    <t>Bolton</t>
-  </si>
-  <si>
-    <t>Boxborough</t>
-  </si>
-  <si>
-    <t>Braintree</t>
-  </si>
-  <si>
-    <t>Burlington</t>
-  </si>
-  <si>
-    <t>Canton</t>
-  </si>
-  <si>
-    <t>Carlisle</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Cohasset</t>
-  </si>
-  <si>
-    <t>Concord</t>
-  </si>
-  <si>
-    <t>Danvers</t>
-  </si>
-  <si>
-    <t>Dedham</t>
-  </si>
-  <si>
-    <t>Dover</t>
-  </si>
-  <si>
-    <t>Essex</t>
-  </si>
-  <si>
-    <t>Foxborough</t>
-  </si>
-  <si>
-    <t>Hamilton</t>
-  </si>
-  <si>
-    <t>Hingham</t>
-  </si>
-  <si>
-    <t>Holbrook</t>
-  </si>
-  <si>
-    <t>Holliston</t>
-  </si>
-  <si>
-    <t>Hopkinton</t>
-  </si>
-  <si>
-    <t>Hull</t>
-  </si>
-  <si>
-    <t>Ipswich</t>
-  </si>
-  <si>
-    <t>Lincoln</t>
-  </si>
-  <si>
-    <t>Littleton</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Lynnfield</t>
-  </si>
-  <si>
-    <t>Manchester</t>
-  </si>
-  <si>
-    <t>Marshfield</t>
-  </si>
-  <si>
-    <t>Maynard</t>
-  </si>
-  <si>
-    <t>Medfield</t>
-  </si>
-  <si>
-    <t>Medway</t>
-  </si>
-  <si>
-    <t>Melrose</t>
-  </si>
-  <si>
-    <t>Middleton</t>
-  </si>
-  <si>
-    <t>Millis</t>
-  </si>
-  <si>
-    <t>Milton</t>
-  </si>
-  <si>
-    <t>Nahant</t>
-  </si>
-  <si>
-    <t>Natick</t>
-  </si>
-  <si>
-    <t>Norfolk</t>
-  </si>
-  <si>
-    <t>North Reading</t>
-  </si>
-  <si>
-    <t>Norwell</t>
-  </si>
-  <si>
-    <t>Norwood</t>
-  </si>
-  <si>
-    <t>Peabody</t>
-  </si>
-  <si>
-    <t>Randolph</t>
-  </si>
-  <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>Rockland</t>
-  </si>
-  <si>
-    <t>Rockport</t>
-  </si>
-  <si>
-    <t>Salem</t>
-  </si>
-  <si>
-    <t>Saugus</t>
-  </si>
-  <si>
-    <t>Scituate</t>
-  </si>
-  <si>
-    <t>Sharon</t>
-  </si>
-  <si>
-    <t>Sherborn</t>
-  </si>
-  <si>
-    <t>Southborough</t>
-  </si>
-  <si>
-    <t>Stoneham</t>
-  </si>
-  <si>
-    <t>Stow</t>
-  </si>
-  <si>
-    <t>Sudbury</t>
-  </si>
-  <si>
-    <t>Swampscott</t>
-  </si>
-  <si>
-    <t>Topsfield</t>
-  </si>
-  <si>
-    <t>Walpole</t>
-  </si>
-  <si>
-    <t>Wayland</t>
-  </si>
-  <si>
-    <t>Wellesley</t>
-  </si>
-  <si>
-    <t>Wenham</t>
-  </si>
-  <si>
-    <t>Weston</t>
-  </si>
-  <si>
-    <t>Westwood</t>
-  </si>
-  <si>
-    <t>Weymouth</t>
-  </si>
-  <si>
-    <t>Wilmington</t>
-  </si>
-  <si>
-    <t>Winchester</t>
-  </si>
-  <si>
-    <t>Winthrop</t>
-  </si>
-  <si>
-    <t>Woburn</t>
-  </si>
-  <si>
-    <t>Wrentham</t>
-  </si>
-  <si>
-    <t>Bicycle/Pedestrian Facility Segment</t>
-  </si>
-  <si>
-    <t>Bicycle/Pedestrian Facility Intersection</t>
-  </si>
-  <si>
-    <t>Street Segment</t>
-  </si>
-  <si>
-    <t>Street Intersection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other (please type in cell to the right)</t>
-  </si>
-  <si>
-    <t>Other (please type in cell to the right)</t>
-  </si>
-  <si>
-    <t>Other (please type in cell below)</t>
-  </si>
-  <si>
-    <t>Bicycle/Pedestrian Facility Name</t>
-  </si>
-  <si>
-    <t>Arthur Fiedler Footbridge</t>
-  </si>
-  <si>
-    <t>Dr. Paul Dudley White Path</t>
-  </si>
-  <si>
-    <t>Salem-Marblehead Trail</t>
-  </si>
-  <si>
-    <t>Southern New England Trunkline Trail</t>
-  </si>
-  <si>
-    <t>Southwest Corridor Park</t>
-  </si>
-  <si>
-    <t>Cleveland Circle - Chestnut Hill Ave at Beacon St</t>
-  </si>
-  <si>
-    <t>Sweetser Circle - Broadway and Bartlett Street</t>
-  </si>
-  <si>
-    <t>Union Square - Washington St between Kingman Rd and Hawkins St</t>
-  </si>
-  <si>
-    <t>Webster Square - Park Avenue at Mill Street</t>
-  </si>
-  <si>
-    <t>Western Avenue Bridge at Memorial Drive</t>
+    <t>Location ID</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1545,15 +1551,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1583,113 +1580,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1698,188 +1590,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1888,166 +1603,58 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2080,10 +1687,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:F273" totalsRowShown="0">
-  <autoFilter ref="D1:F273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:G273" totalsRowShown="0">
+  <autoFilter ref="D1:G273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{09935779-A7F4-4E95-BF0B-6D7F0A5AF862}" name="Count Location Description"/>
+    <tableColumn id="2" xr3:uid="{881AF884-5F10-4B59-94B7-B2F4180F93D0}" name="Location ID"/>
     <tableColumn id="4" xr3:uid="{C9E4663B-CFA0-49B0-ABFE-EA028F045F02}" name="Sky"/>
     <tableColumn id="5" xr3:uid="{DDD78CD7-2084-4F6C-8D99-B7CB3992BAA4}" name="Direction"/>
   </tableColumns>
@@ -2388,255 +1996,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D396DD5C-31B0-418A-83C6-51CCF2B5706A}">
-  <dimension ref="B1:N14"/>
+  <dimension ref="B1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="1" width="1.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="5" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="2:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>305</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="I2" s="37" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="21"/>
+      <c r="J2" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
-    </row>
-    <row r="3" spans="2:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
-    </row>
-    <row r="4" spans="2:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="21"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45"/>
-    </row>
-    <row r="5" spans="2:14" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="16"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
-    </row>
-    <row r="6" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="57"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="48"/>
-    </row>
-    <row r="7" spans="2:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="35" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="1">
+        <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
+        <v>20179</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="57"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="48"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="48"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="35" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="48"/>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="35" t="s">
-        <v>427</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="51"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="1"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="52" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-    </row>
-    <row r="14" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="1"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="26">
+    <mergeCell ref="J2:O3"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D2:E4"/>
+    <mergeCell ref="F2:G4"/>
+    <mergeCell ref="J4:O12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="I2:N3"/>
-    <mergeCell ref="I4:N10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="F2:G5"/>
-    <mergeCell ref="D2:E5"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">
       <formula1>-100</formula1>
       <formula2>120</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 D12:G12 D13:G13" xr:uid="{90E49F85-3C5D-4AFE-BE6F-92C7D2ED3A5A}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D7:H7 D9:H9" xr:uid="{90E49F85-3C5D-4AFE-BE6F-92C7D2ED3A5A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2646,23 +2270,23 @@
           <x14:formula1>
             <xm:f>Columns!$D$2:$D$272</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:E6</xm:sqref>
+          <xm:sqref>D5:E5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{5083652B-750A-4C4D-B750-005AF92A196B}">
           <x14:formula1>
             <xm:f>Columns!$C$2:$C$37</xm:f>
           </x14:formula1>
-          <xm:sqref>D7:E7</xm:sqref>
+          <xm:sqref>D6:E7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{58E12AA0-633A-41A0-A830-DA54E1AC4088}">
           <x14:formula1>
-            <xm:f>Columns!$F$2:$F$7</xm:f>
+            <xm:f>Columns!$G$2:$G$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:E8 D9:E9</xm:sqref>
+          <xm:sqref>D8:E10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{300277EC-7D8D-4617-9225-79CC1A5F70F0}">
           <x14:formula1>
-            <xm:f>Columns!$E$2:$E$7</xm:f>
+            <xm:f>Columns!$F$2:$F$7</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
@@ -2670,13 +2294,13 @@
           <x14:formula1>
             <xm:f>Columns!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:E10 D10:E10</xm:sqref>
+          <xm:sqref>D11:E11 D11:E11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E9B4B24B-D1FA-4151-8197-DA5E2D5B65FD}">
           <x14:formula1>
             <xm:f>Columns!$A$2:$A$99</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:E11</xm:sqref>
+          <xm:sqref>D12:E12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3228,10 +2852,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92867D1-D2E9-42B4-B903-CE81613CFB5C}">
-  <dimension ref="A1:F272"/>
+  <dimension ref="A1:G272"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,7 +2870,7 @@
     <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3254,44 +2878,47 @@
         <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D1" t="s">
         <v>66</v>
       </c>
       <c r="E1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F1" t="s">
         <v>321</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F2" t="s">
         <v>326</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -3299,19 +2926,22 @@
       <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9">
+        <v>20260</v>
+      </c>
+      <c r="F3" t="s">
         <v>327</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -3319,39 +2949,45 @@
       <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9">
+        <v>20240</v>
+      </c>
+      <c r="F4" t="s">
         <v>328</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D5" t="s">
         <v>69</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9">
+        <v>20173</v>
+      </c>
+      <c r="F5" t="s">
         <v>329</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -3359,16 +2995,19 @@
       <c r="D6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9">
+        <v>20179</v>
+      </c>
+      <c r="F6" t="s">
         <v>330</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -3376,14 +3015,17 @@
       <c r="D7" t="s">
         <v>332</v>
       </c>
-      <c r="E7" t="s">
-        <v>432</v>
+      <c r="E7" s="9">
+        <v>20284</v>
       </c>
       <c r="F7" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="G7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3393,10 +3035,13 @@
       <c r="D8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="9">
+        <v>20283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -3404,10 +3049,13 @@
       <c r="D9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="9">
+        <v>20192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -3415,8 +3063,11 @@
       <c r="D10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="9">
+        <v>20125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3426,10 +3077,13 @@
       <c r="D11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="9">
+        <v>10037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -3437,10 +3091,13 @@
       <c r="D12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="9">
+        <v>20047</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -3448,8 +3105,11 @@
       <c r="D13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="9">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -3459,19 +3119,25 @@
       <c r="D14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="9">
+        <v>20041</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D15" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="9">
+        <v>20276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3481,10 +3147,13 @@
       <c r="D16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="9">
+        <v>20063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -3492,10 +3161,13 @@
       <c r="D17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="9">
+        <v>10460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C18" t="s">
         <v>46</v>
@@ -3503,10 +3175,13 @@
       <c r="D18" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="9">
+        <v>20203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
@@ -3514,10 +3189,13 @@
       <c r="D19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="9">
+        <v>20211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -3525,10 +3203,13 @@
       <c r="D20" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="9">
+        <v>20216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C21" t="s">
         <v>49</v>
@@ -3536,10 +3217,13 @@
       <c r="D21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="9">
+        <v>20206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
@@ -3547,10 +3231,13 @@
       <c r="D22" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="9">
+        <v>10528</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C23" t="s">
         <v>51</v>
@@ -3558,10 +3245,13 @@
       <c r="D23" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="9">
+        <v>20077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C24" t="s">
         <v>52</v>
@@ -3569,10 +3259,13 @@
       <c r="D24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="9">
+        <v>20228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C25" t="s">
         <v>53</v>
@@ -3580,8 +3273,11 @@
       <c r="D25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="9">
+        <v>20163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -3591,10 +3287,13 @@
       <c r="D26" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="9">
+        <v>20013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C27" t="s">
         <v>55</v>
@@ -3602,8 +3301,11 @@
       <c r="D27" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="9">
+        <v>20218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -3613,19 +3315,25 @@
       <c r="D28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="9">
+        <v>20257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D29" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="9">
+        <v>20251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -3635,10 +3343,13 @@
       <c r="D30" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="9">
+        <v>20038</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C31" t="s">
         <v>60</v>
@@ -3646,10 +3357,13 @@
       <c r="D31" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="9">
+        <v>20134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C32" t="s">
         <v>61</v>
@@ -3657,32 +3371,41 @@
       <c r="D32" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="9">
+        <v>20109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C33" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="9">
+        <v>20225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C34" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D34" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="9">
+        <v>20014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C35" t="s">
         <v>62</v>
@@ -3690,8 +3413,11 @@
       <c r="D35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="9">
+        <v>20137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -3701,10 +3427,13 @@
       <c r="D36" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="9">
+        <v>20112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C37" t="s">
         <v>64</v>
@@ -3712,1366 +3441,2074 @@
       <c r="D37" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="9">
+        <v>20249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D38" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="9">
+        <v>20023</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
       <c r="D39" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="9">
+        <v>20102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D40" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="9">
+        <v>20207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D41" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="9">
+        <v>20201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D42" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="9">
+        <v>20217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D43" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="9">
+        <v>20142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
       <c r="D44" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="9">
+        <v>20143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>20144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
       <c r="D46" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="9">
+        <v>20176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="D47" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="9">
+        <v>20155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D48" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="9">
+        <v>20199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D49" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="9">
+        <v>20182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D50" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="9">
+        <v>20227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
       <c r="D51" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="9">
+        <v>20231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D52" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="9">
+        <v>20098</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D53" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="9">
+        <v>20156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D54" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="9">
+        <v>20157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="D55" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="9">
+        <v>20247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D56" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="9">
+        <v>11044</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D57" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="9">
+        <v>20209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D58" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="9">
+        <v>20278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D59" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="9">
+        <v>20095</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
       <c r="D60" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="9">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="9">
+        <v>20256</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D62" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+      <c r="E62" s="9">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D63" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="9">
+        <v>20161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D64" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="9">
+        <v>20197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D65" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="9">
+        <v>20078</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D66" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="9">
+        <v>20279</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>21</v>
       </c>
       <c r="D67" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="9">
+        <v>20190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D68" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="9">
+        <v>20214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D69" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="9">
+        <v>20239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
       <c r="D70" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="9">
+        <v>20210</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D71" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="9">
+        <v>20264</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D72" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="9">
+        <v>10970</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D73" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="9">
+        <v>20267</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D74" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="9">
+        <v>20265</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D75" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="9">
+        <v>20277</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D76" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="9">
+        <v>20099</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D77" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="9">
+        <v>20066</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>23</v>
       </c>
       <c r="D78" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="9">
+        <v>20233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D79" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="9">
+        <v>20224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D80" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="9">
+        <v>20229</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D81" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="9">
+        <v>20186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D82" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="9">
+        <v>20141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D83" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="9">
+        <v>20243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D84" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="9">
+        <v>20016</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
       <c r="D85" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="9">
+        <v>20270</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D86" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="9">
+        <v>20261</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>25</v>
       </c>
       <c r="D87" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="9">
+        <v>20258</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>26</v>
       </c>
       <c r="D88" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="9">
+        <v>20075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D89" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="9">
+        <v>20087</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D90" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="9">
+        <v>20079</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D91" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="9">
+        <v>20140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D92" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="9">
+        <v>20238</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D93" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="9">
+        <v>20262</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D94" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="9">
+        <v>20236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D95" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="9">
+        <v>20222</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D96" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="9">
+        <v>20174</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D97" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="9">
+        <v>20120</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D98" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="9">
+        <v>20091</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D99" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="9">
+        <v>20015</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="9">
+        <v>20127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="9">
+        <v>20040</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="9">
+        <v>20031</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="9">
+        <v>20168</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="9">
+        <v>20080</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="9">
+        <v>20275</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="9">
+        <v>20266</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="9">
+        <v>20085</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="9">
+        <v>20113</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="9">
+        <v>20183</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="9">
+        <v>20181</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="9">
+        <v>20172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="9">
+        <v>20193</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="9">
+        <v>20122</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="9">
+        <v>10782</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="9">
+        <v>20050</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="9">
+        <v>20241</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="9">
+        <v>10029</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="9">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="9">
+        <v>20132</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="9">
+        <v>20110</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="9">
+        <v>20135</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="9">
+        <v>20019</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="9">
+        <v>20166</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="9">
+        <v>20198</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="9">
+        <v>20138</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="9">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="9">
+        <v>20034</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="9">
+        <v>20030</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="9">
+        <v>20025</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="9">
+        <v>20124</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="9">
+        <v>11058</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="9">
+        <v>20121</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="9">
+        <v>20189</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="9">
+        <v>10127</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="9">
+        <v>20018</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="9">
+        <v>20259</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="9">
+        <v>20026</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="9">
+        <v>11048</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="9">
+        <v>20131</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="9">
+        <v>20036</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="9">
+        <v>20035</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="9">
+        <v>20133</v>
+      </c>
+    </row>
+    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="9">
+        <v>20130</v>
+      </c>
+    </row>
+    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="9">
+        <v>20106</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="9">
+        <v>20027</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="9">
+        <v>20271</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="9">
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="9">
+        <v>20052</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="9">
+        <v>10713</v>
+      </c>
+    </row>
+    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="9">
+        <v>20212</v>
+      </c>
+    </row>
+    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="9">
+        <v>11015</v>
+      </c>
+    </row>
+    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="9">
+        <v>20171</v>
+      </c>
+    </row>
+    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="9">
+        <v>20042</v>
+      </c>
+    </row>
+    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="9">
+        <v>20226</v>
+      </c>
+    </row>
+    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="9">
+        <v>20043</v>
+      </c>
+    </row>
+    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="9">
+        <v>20269</v>
+      </c>
+    </row>
+    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="9">
+        <v>20223</v>
+      </c>
+    </row>
+    <row r="158" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="9">
+        <v>20268</v>
+      </c>
+    </row>
+    <row r="159" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="9">
+        <v>20215</v>
+      </c>
+    </row>
+    <row r="160" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="9">
+        <v>20008</v>
+      </c>
+    </row>
+    <row r="161" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="9">
+        <v>20097</v>
+      </c>
+    </row>
+    <row r="162" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="9">
+        <v>10432</v>
+      </c>
+    </row>
+    <row r="163" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="9">
+        <v>20048</v>
+      </c>
+    </row>
+    <row r="164" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="9">
+        <v>20175</v>
+      </c>
+    </row>
+    <row r="165" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="9">
+        <v>20051</v>
+      </c>
+    </row>
+    <row r="166" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="9">
+        <v>20039</v>
+      </c>
+    </row>
+    <row r="167" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="9">
+        <v>20230</v>
+      </c>
+    </row>
+    <row r="168" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="9">
+        <v>20196</v>
+      </c>
+    </row>
+    <row r="169" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="9">
+        <v>20221</v>
+      </c>
+    </row>
+    <row r="170" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="9">
+        <v>20188</v>
+      </c>
+    </row>
+    <row r="171" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="9">
+        <v>20054</v>
+      </c>
+    </row>
+    <row r="172" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="9">
+        <v>20032</v>
+      </c>
+    </row>
+    <row r="173" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="9">
+        <v>20010</v>
+      </c>
+    </row>
+    <row r="174" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="9">
+        <v>20055</v>
+      </c>
+    </row>
+    <row r="175" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="9">
+        <v>20061</v>
+      </c>
+    </row>
+    <row r="176" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D176" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="9">
+        <v>20056</v>
+      </c>
+    </row>
+    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="9">
+        <v>20057</v>
+      </c>
+    </row>
+    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="9">
+        <v>20060</v>
+      </c>
+    </row>
+    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="9">
+        <v>20003</v>
+      </c>
+    </row>
+    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="9">
+        <v>20058</v>
+      </c>
+    </row>
+    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="9">
+        <v>20005</v>
+      </c>
+    </row>
+    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="9">
+        <v>20033</v>
+      </c>
+    </row>
+    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D183" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="9">
+        <v>20128</v>
+      </c>
+    </row>
+    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D184" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="9">
+        <v>20009</v>
+      </c>
+    </row>
+    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D185" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="9">
+        <v>20006</v>
+      </c>
+    </row>
+    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="9">
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="9">
+        <v>20007</v>
+      </c>
+    </row>
+    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="9">
+        <v>20059</v>
+      </c>
+    </row>
+    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="9">
+        <v>20145</v>
+      </c>
+    </row>
+    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="9">
+        <v>20096</v>
+      </c>
+    </row>
+    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="9">
+        <v>11073</v>
+      </c>
+    </row>
+    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="9">
+        <v>20234</v>
+      </c>
+    </row>
+    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E193" s="9">
+        <v>20017</v>
+      </c>
+    </row>
+    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E194" s="9">
+        <v>20073</v>
+      </c>
+    </row>
+    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E195" s="9">
+        <v>20011</v>
+      </c>
+    </row>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="9">
+        <v>20046</v>
+      </c>
+    </row>
+    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E197" s="9">
+        <v>20194</v>
+      </c>
+    </row>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D198" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E198" s="9">
+        <v>20139</v>
+      </c>
+    </row>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E199" s="9">
+        <v>10471</v>
+      </c>
+    </row>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E200" s="9">
+        <v>10983</v>
+      </c>
+    </row>
+    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E201" s="9">
+        <v>20068</v>
+      </c>
+    </row>
+    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E202" s="9">
+        <v>20069</v>
+      </c>
+    </row>
+    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E203" s="9">
+        <v>20274</v>
+      </c>
+    </row>
+    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E204" s="9">
+        <v>20232</v>
+      </c>
+    </row>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E205" s="9">
+        <v>20071</v>
+      </c>
+    </row>
+    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E206" s="9">
+        <v>20280</v>
+      </c>
+    </row>
+    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E207" s="9">
+        <v>20170</v>
+      </c>
+    </row>
+    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E208" s="9">
+        <v>20072</v>
+      </c>
+    </row>
+    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D209" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E209" s="9">
+        <v>20147</v>
+      </c>
+    </row>
+    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="9">
+        <v>20204</v>
+      </c>
+    </row>
+    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E211" s="9">
+        <v>20165</v>
+      </c>
+    </row>
+    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E212" s="9">
+        <v>20237</v>
+      </c>
+    </row>
+    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E213" s="9">
+        <v>20028</v>
+      </c>
+    </row>
+    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E214" s="9">
+        <v>20242</v>
+      </c>
+    </row>
+    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E215" s="9">
+        <v>20076</v>
+      </c>
+    </row>
+    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D216" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E216" s="9">
+        <v>20020</v>
+      </c>
+    </row>
+    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D217" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E217" s="9">
+        <v>20253</v>
+      </c>
+    </row>
+    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E218" s="9">
+        <v>20022</v>
+      </c>
+    </row>
+    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E219" s="9">
+        <v>20169</v>
+      </c>
+    </row>
+    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E220" s="9">
+        <v>20146</v>
+      </c>
+    </row>
+    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E221" s="9">
+        <v>20105</v>
+      </c>
+    </row>
+    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D222" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E222" s="9">
+        <v>20282</v>
+      </c>
+    </row>
+    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D223" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E223" s="9">
+        <v>20281</v>
+      </c>
+    </row>
+    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D224" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="9">
+        <v>20062</v>
+      </c>
+    </row>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="9">
+        <v>20148</v>
+      </c>
+    </row>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D226" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E226" s="9">
+        <v>20202</v>
+      </c>
+    </row>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D227" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="9">
+        <v>20191</v>
+      </c>
+    </row>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D228" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="9">
+        <v>20220</v>
+      </c>
+    </row>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D229" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="9">
+        <v>20255</v>
+      </c>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D230" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E230" s="9">
+        <v>20185</v>
+      </c>
+    </row>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D231" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E231" s="9">
+        <v>20044</v>
+      </c>
+    </row>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D232" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E232" s="9">
+        <v>20160</v>
+      </c>
+    </row>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D233" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E233" s="9">
+        <v>20159</v>
+      </c>
+    </row>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D234" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E234" s="9">
+        <v>20081</v>
+      </c>
+    </row>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D235" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E235" s="9">
+        <v>20252</v>
+      </c>
+    </row>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D236" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E236" s="9">
+        <v>20114</v>
+      </c>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D237" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E237" s="9">
+        <v>20149</v>
+      </c>
+    </row>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D238" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E238" s="9">
+        <v>20187</v>
+      </c>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D239" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E239" s="9">
+        <v>20115</v>
+      </c>
+    </row>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E240" s="9">
+        <v>20184</v>
+      </c>
+    </row>
+    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E241" s="9">
+        <v>20245</v>
+      </c>
+    </row>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E242" s="9">
+        <v>20246</v>
+      </c>
+    </row>
+    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+      <c r="E243" s="9">
+        <v>20180</v>
+      </c>
+    </row>
+    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E244" s="9">
+        <v>20235</v>
+      </c>
+    </row>
+    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E245" s="9">
+        <v>20177</v>
+      </c>
+    </row>
+    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D246" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E246" s="9">
+        <v>20093</v>
+      </c>
+    </row>
+    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E247" s="9">
+        <v>20116</v>
+      </c>
+    </row>
+    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E248" s="9">
+        <v>10202</v>
+      </c>
+    </row>
+    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E249" s="9">
+        <v>20074</v>
+      </c>
+    </row>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+      <c r="E250" s="9">
+        <v>20123</v>
+      </c>
+    </row>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D251" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E251" s="9">
+        <v>20064</v>
+      </c>
+    </row>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E252" s="9">
+        <v>20065</v>
+      </c>
+    </row>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D253" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E253" s="9">
+        <v>20178</v>
+      </c>
+    </row>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E254" s="9">
+        <v>20200</v>
+      </c>
+    </row>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E255" s="9">
+        <v>20254</v>
+      </c>
+    </row>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E256" s="9">
+        <v>20248</v>
+      </c>
+    </row>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E257" s="9">
+        <v>20219</v>
+      </c>
+    </row>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D258" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E258" s="9">
+        <v>20244</v>
+      </c>
+    </row>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D259" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E259" s="9">
+        <v>20263</v>
+      </c>
+    </row>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D260" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E260" s="9">
+        <v>10012</v>
+      </c>
+    </row>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D261" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E261" s="9">
+        <v>20117</v>
+      </c>
+    </row>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D262" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E262" s="9">
+        <v>10048</v>
+      </c>
+    </row>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D263" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+      <c r="E263" s="9">
+        <v>20164</v>
+      </c>
+    </row>
+    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D264" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E264" s="9">
+        <v>20272</v>
+      </c>
+    </row>
+    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D265" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E265" s="9">
+        <v>20012</v>
+      </c>
+    </row>
+    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E266" s="9">
+        <v>20208</v>
+      </c>
+    </row>
+    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D267" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+      <c r="E267" s="9">
+        <v>20021</v>
+      </c>
+    </row>
+    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E268" s="9">
+        <v>20273</v>
+      </c>
+    </row>
+    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D269" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E269" s="9">
+        <v>20082</v>
+      </c>
+    </row>
+    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D270" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E270" s="9">
+        <v>20205</v>
+      </c>
+    </row>
+    <row r="271" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E271" s="9">
+        <v>20118</v>
+      </c>
+    </row>
+    <row r="272" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
         <v>303</v>
+      </c>
+      <c r="E272" s="9">
+        <v>20195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>